<commit_message>
Add Nucleo_DCO_Test19 (ADC Off)
</commit_message>
<xml_diff>
--- a/Nucleo_DCO_ブロック図.xlsx
+++ b/Nucleo_DCO_ブロック図.xlsx
@@ -84,15 +84,15 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>9V Power</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>3.3V Power</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>2018.09.21</t>
+    <t>2018.09.25</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>DC9VIN</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -180,15 +180,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>152868</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>172640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>60</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>172640</xdr:rowOff>
+      <xdr:colOff>152867</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>1189</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>64</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -197,8 +197,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7996498" y="2607727"/>
-          <a:ext cx="2456154" cy="1391478"/>
+          <a:off x="7794034" y="2541189"/>
+          <a:ext cx="3064466" cy="2369479"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -484,16 +484,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>174170</xdr:colOff>
       <xdr:row>16</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>26</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>174171</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -502,8 +502,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1899047" y="2762250"/>
-          <a:ext cx="2589609" cy="1035844"/>
+          <a:off x="870856" y="2786743"/>
+          <a:ext cx="3657601" cy="1045028"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -882,15 +882,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>41</xdr:col>
-      <xdr:colOff>16564</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>1190</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>9267</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>45</xdr:col>
-      <xdr:colOff>16565</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>1190</xdr:rowOff>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9267</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -899,8 +899,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="7147890" y="3479886"/>
-          <a:ext cx="712305" cy="695739"/>
+          <a:off x="6942667" y="2887934"/>
+          <a:ext cx="698501" cy="677333"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -1458,8 +1458,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>46</xdr:col>
-      <xdr:colOff>152868</xdr:colOff>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>16565</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
@@ -1470,8 +1470,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6783457" y="3304761"/>
-          <a:ext cx="1386976" cy="0"/>
+          <a:off x="6604000" y="3217333"/>
+          <a:ext cx="355232" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1499,26 +1499,29 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>161693</xdr:colOff>
+      <xdr:col>45</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>42</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>12604</xdr:rowOff>
+      <xdr:rowOff>6134</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>46</xdr:col>
+      <xdr:colOff>152868</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9268</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
         <xdr:cNvPr id="39" name="Straight Arrow Connector 38"/>
-        <xdr:cNvCxnSpPr/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="13" idx="6"/>
+          <a:endCxn id="19" idx="1"/>
+        </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipH="1" flipV="1">
-          <a:off x="7381643" y="3257550"/>
-          <a:ext cx="232" cy="184054"/>
+        <a:xfrm flipV="1">
+          <a:off x="7641168" y="3223467"/>
+          <a:ext cx="322200" cy="3134"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2958,16 +2961,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
+      <xdr:col>11</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>172640</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>165157</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>166688</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2976,8 +2979,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2071688" y="2934890"/>
-          <a:ext cx="690562" cy="690563"/>
+          <a:off x="1915886" y="2951900"/>
+          <a:ext cx="696686" cy="698217"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3006,7 +3009,14 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0"/>
-            <a:t>Reseve SW</a:t>
+            <a:t>ADC Off </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0"/>
+            <a:t>SW</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
         </a:p>
@@ -3127,15 +3137,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>39</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>2304</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>2304</xdr:colOff>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -3145,8 +3155,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5829300" y="5143500"/>
-          <a:ext cx="857250" cy="514350"/>
+          <a:off x="8998137" y="4233333"/>
+          <a:ext cx="846667" cy="508000"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3187,14 +3197,14 @@
     <xdr:from>
       <xdr:col>28</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>161927</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3203,8 +3213,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="4782207" y="3586655"/>
-          <a:ext cx="341586" cy="2"/>
+          <a:off x="4800600" y="4791075"/>
+          <a:ext cx="342900" cy="2"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3232,16 +3242,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>28</xdr:col>
+      <xdr:col>48</xdr:col>
       <xdr:colOff>2</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>2</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>89428</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>112643</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3251,9 +3261,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm rot="16200000" flipH="1">
-          <a:off x="4069558" y="4331496"/>
-          <a:ext cx="1804986" cy="342898"/>
+        <a:xfrm rot="5400000" flipH="1" flipV="1">
+          <a:off x="7318870" y="5322394"/>
+          <a:ext cx="1773239" cy="112641"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -3278,16 +3288,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>112643</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9523</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>112643</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>169331</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3296,8 +3306,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm flipH="1">
-          <a:off x="5143500" y="5153025"/>
-          <a:ext cx="514350" cy="504825"/>
+          <a:off x="8261810" y="4242856"/>
+          <a:ext cx="508000" cy="498475"/>
         </a:xfrm>
         <a:prstGeom prst="homePlate">
           <a:avLst/>
@@ -3336,16 +3346,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>34</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>90488</xdr:rowOff>
+      <xdr:col>51</xdr:col>
+      <xdr:colOff>112643</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>2304</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>89427</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3357,8 +3367,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="5657850" y="5400675"/>
-          <a:ext cx="171450" cy="4763"/>
+          <a:off x="8769810" y="4487333"/>
+          <a:ext cx="228327" cy="4761"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -3383,65 +3393,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>145676</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="Straight Arrow Connector 55"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="51" idx="0"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6257925" y="4431926"/>
-          <a:ext cx="0" cy="711574"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>165157</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>9526</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>165158</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3450,8 +3411,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2876550" y="2944416"/>
-          <a:ext cx="690563" cy="690563"/>
+          <a:off x="2786743" y="2951900"/>
+          <a:ext cx="696686" cy="696687"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3502,15 +3463,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>21</xdr:col>
-      <xdr:colOff>41672</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>8595</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>25</xdr:col>
-      <xdr:colOff>41672</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>166688</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>8595</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -3519,8 +3480,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3667125" y="2928938"/>
-          <a:ext cx="690563" cy="690563"/>
+          <a:off x="3657600" y="2969509"/>
+          <a:ext cx="696686" cy="696686"/>
         </a:xfrm>
         <a:prstGeom prst="ellipse">
           <a:avLst/>
@@ -3724,7 +3685,7 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>63</xdr:col>
+      <xdr:col>67</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>13</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
@@ -3737,7 +3698,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7391400" y="1200150"/>
-          <a:ext cx="3429000" cy="1028700"/>
+          <a:ext cx="4114800" cy="1028700"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
           <a:avLst/>
@@ -3851,7 +3812,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
-            <a:t>Vald</a:t>
+            <a:t>Valid</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
         </a:p>
@@ -3916,7 +3877,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
-            <a:t>Vald</a:t>
+            <a:t>Valid</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
         </a:p>
@@ -3981,7 +3942,7 @@
           <a:pPr algn="ctr"/>
           <a:r>
             <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
-            <a:t>Vald</a:t>
+            <a:t>Valid</a:t>
           </a:r>
           <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
         </a:p>
@@ -4149,16 +4110,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>58</xdr:col>
+      <xdr:col>62</xdr:col>
       <xdr:colOff>152400</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>64</xdr:col>
+      <xdr:rowOff>9268</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>9268</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4167,8 +4128,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10257183" y="3304761"/>
-          <a:ext cx="891208" cy="0"/>
+          <a:off x="10672233" y="3226601"/>
+          <a:ext cx="863600" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4197,65 +4158,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>39</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>1190</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>52</xdr:col>
-      <xdr:colOff>162159</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:cxnSp macro="">
-      <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="76" name="Elbow Connector 75"/>
-        <xdr:cNvCxnSpPr>
-          <a:stCxn id="51" idx="3"/>
-          <a:endCxn id="73" idx="2"/>
-        </xdr:cNvCxnSpPr>
-      </xdr:nvCxnSpPr>
-      <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="6686550" y="3944540"/>
-          <a:ext cx="2410059" cy="2656285"/>
-        </a:xfrm>
-        <a:prstGeom prst="bentConnector2">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:ln>
-          <a:tailEnd type="triangle"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="3">
-          <a:schemeClr val="accent6"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent6"/>
-        </a:fillRef>
-        <a:effectRef idx="2">
-          <a:schemeClr val="accent6"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:cxnSp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>39</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>42</xdr:col>
-      <xdr:colOff>161925</xdr:colOff>
+      <xdr:colOff>160940</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4266,8 +4177,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="6696075" y="4972050"/>
-          <a:ext cx="685800" cy="409575"/>
+          <a:off x="6670456" y="4953000"/>
+          <a:ext cx="683501" cy="341587"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
           <a:avLst/>
@@ -4291,6 +4202,429 @@
         </a:fontRef>
       </xdr:style>
     </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>150451</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>38101</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>151982</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="74" name="Oval 73"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1083129" y="2937194"/>
+          <a:ext cx="696686" cy="698217"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800" baseline="0"/>
+            <a:t>Reseve SW</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>61</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>66</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="78" name="Oval 77"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10648949" y="1381125"/>
+          <a:ext cx="685801" cy="685800"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
+            <a:t>ADC</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="800"/>
+            <a:t>Valid</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="800"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="80" name="Elbow Connector 79"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="16200000" flipH="1">
+          <a:off x="4013639" y="5550775"/>
+          <a:ext cx="1537138" cy="2"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="86" name="Straight Connector 85"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4782209" y="6319345"/>
+          <a:ext cx="3435567" cy="0"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>11834</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>169332</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>55</xdr:col>
+      <xdr:colOff>86972</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>160734</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="91" name="Elbow Connector 90"/>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="51" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="5400000">
+          <a:off x="7684285" y="3672881"/>
+          <a:ext cx="668735" cy="2805638"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>84666</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>68</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>89428</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="99" name="Straight Arrow Connector 98"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9842501" y="4487333"/>
+          <a:ext cx="1693332" cy="4762"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>160735</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="105" name="Rounded Rectangle 104"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8995833" y="3716735"/>
+          <a:ext cx="846667" cy="516598"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent6">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>VGND</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>58</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>20599</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>62</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>15675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="108" name="Pentagon 107"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9994900" y="2899266"/>
+          <a:ext cx="677333" cy="672409"/>
+        </a:xfrm>
+        <a:prstGeom prst="homePlate">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+            <a:t>AC Cpl</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -4562,10 +4896,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:BJ40"/>
+  <dimension ref="B2:BN38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="BR40" sqref="A1:BR40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.25" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4590,7 +4924,7 @@
     </row>
     <row r="3" spans="2:42" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="2:42" x14ac:dyDescent="0.15">
@@ -4598,50 +4932,50 @@
         <v>8</v>
       </c>
       <c r="AP12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="28:66" x14ac:dyDescent="0.15">
+      <c r="BN20" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="21" spans="28:66" x14ac:dyDescent="0.15">
+      <c r="AB21">
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="28:62" x14ac:dyDescent="0.15">
-      <c r="BJ20" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="21" spans="28:62" x14ac:dyDescent="0.15">
-      <c r="AB21">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="25" spans="28:62" x14ac:dyDescent="0.15">
-      <c r="BC25" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="28:62" x14ac:dyDescent="0.15">
+    <row r="27" spans="28:66" x14ac:dyDescent="0.15">
       <c r="AB27" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="31" spans="28:62" x14ac:dyDescent="0.15">
-      <c r="AR31" t="s">
-        <v>11</v>
+    <row r="28" spans="28:66" x14ac:dyDescent="0.15">
+      <c r="BN28" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="33" spans="26:62" x14ac:dyDescent="0.15">
+    <row r="31" spans="28:66" x14ac:dyDescent="0.15">
+      <c r="AR31" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="32:62" x14ac:dyDescent="0.15">
       <c r="BJ33" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="26:62" x14ac:dyDescent="0.15">
+    <row r="34" spans="32:62" x14ac:dyDescent="0.15">
       <c r="BJ34" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="26:62" x14ac:dyDescent="0.15">
+    <row r="35" spans="32:62" x14ac:dyDescent="0.15">
       <c r="BJ35" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="26:62" x14ac:dyDescent="0.15">
+    <row r="36" spans="32:62" x14ac:dyDescent="0.15">
       <c r="AF36" t="s">
         <v>6</v>
       </c>
@@ -4649,8 +4983,8 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="26:62" x14ac:dyDescent="0.15">
-      <c r="Z40" t="s">
+    <row r="38" spans="32:62" x14ac:dyDescent="0.15">
+      <c r="AJ38" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>